<commit_message>
multicore funcionando com o norm antigo
tem que ajeitar os processadores pra ficar 144 no total, e colocar uns MLT -1 pro out demorar mais um pouquinho e sincronizar
</commit_message>
<xml_diff>
--- a/multicore.xlsx
+++ b/multicore.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melis\Desktop\GitDesk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52653EE-26B1-464C-8488-82A95C9996FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E09514-B613-42F3-A997-C81D4464B939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="481" activeTab="4" xr2:uid="{7C13D048-D369-4CF7-941B-2AB5863FD600}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="481" xr2:uid="{7C13D048-D369-4CF7-941B-2AB5863FD600}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -169,6 +169,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4635,247 +4636,12 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Planilha3!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Processadores</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="110000"/>
-                    <a:satMod val="105000"/>
-                    <a:tint val="67000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="103000"/>
-                    <a:tint val="73000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="105000"/>
-                    <a:satMod val="109000"/>
-                    <a:tint val="81000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Planilha3!$A$2:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>520</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>560</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>640</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>680</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>720</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>760</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>840</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>880</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>920</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>960</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Planilha3!$B$2:$B$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>147</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8010-49B1-82F5-0F03F54BC62B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="247"/>
-        <c:axId val="110171312"/>
-        <c:axId val="85434416"/>
-      </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Planilha3!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Tempo de Atraso</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
+          <c:order val="0"/>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
               <a:solidFill>
@@ -4926,77 +4692,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha3!$F$2:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha3!$C$2:$C$23</c:f>
+              <c:f>Planilha3!$G$2:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>389.64375000000001</c:v>
+                  <c:v>16.212379662449301</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>311.73500000000001</c:v>
+                  <c:v>6.1994799217063896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>260.09997300000003</c:v>
+                  <c:v>6.4429156459154902</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>224.80381999999997</c:v>
+                  <c:v>3.4009593119310302</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>197.62812500000001</c:v>
+                  <c:v>2.4363095817896099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175.94463000000002</c:v>
+                  <c:v>2.1643141369056398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>159.66249999999999</c:v>
+                  <c:v>2.1967323589023602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>143.42402699999997</c:v>
+                  <c:v>2.15821763569675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>132.57285399999998</c:v>
+                  <c:v>2.19944143780836</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>121.62181199999999</c:v>
+                  <c:v>2.18471846914899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>113.48065399999999</c:v>
+                  <c:v>2.1986445153728802</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>108.083279</c:v>
+                  <c:v>2.20296187623845</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>99.992925</c:v>
+                  <c:v>2.1994092317612699</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>94.586770999999999</c:v>
+                  <c:v>2.20021136956119</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>89.166854999999998</c:v>
+                  <c:v>2.2008451582039701</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>86.473043999999987</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>81.058750000000003</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>78.392810999999995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>72.937412999999992</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>70.260419000000013</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>67.631009999999989</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>64.954999999999998</c:v>
+                  <c:v>2.2006481796600599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5004,7 +4809,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8010-49B1-82F5-0F03F54BC62B}"/>
+              <c16:uniqueId val="{00000001-6C8F-4333-9712-759F6D127EC3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5018,8 +4823,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93125648"/>
-        <c:axId val="115242624"/>
+        <c:axId val="110171312"/>
+        <c:axId val="85434416"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="110171312"/>
@@ -5028,6 +4833,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ÍNDICE DO GANHO</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5036,9 +4896,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="accent2">
+                <a:alpha val="0"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -5106,6 +4965,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>RMS DO ERRO</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5140,66 +5054,9 @@
         <c:crossAx val="110171312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
-      <c:valAx>
-        <c:axId val="115242624"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="93125648"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:catAx>
-        <c:axId val="93125648"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115242624"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5208,47 +5065,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.3413300524934384"/>
-          <c:y val="0.144096675415573"/>
-          <c:w val="0.53618131749924702"/>
-          <c:h val="7.4503832716274712E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -5288,8 +5104,9 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -11928,27 +11745,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76094FA6-CFFE-423A-9084-DAE44995ED44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E258BBC5-5F6C-47C2-8892-EDC51E814A5E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -11966,6 +11785,49 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.29842</cdr:x>
+      <cdr:y>0.87153</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.48814</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="CaixaDeTexto 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1A6FBAD-9177-4579-933E-23D9AAF26606}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1438275" y="2390774"/>
+          <a:ext cx="914400" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12008,7 +11870,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -12051,7 +11913,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -12094,7 +11956,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -12436,7 +12298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104259CF-4DA1-435F-859F-CDADF407460C}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -14907,19 +14769,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BA3D75-590D-4E01-9070-2E13EF8BFE53}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E23" sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -14942,7 +14808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>160</v>
       </c>
@@ -14965,7 +14831,7 @@
         <v>16.212379662449301</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>200</v>
       </c>
@@ -14987,8 +14853,17 @@
       <c r="G3" s="8">
         <v>6.1994799217063896</v>
       </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>240</v>
       </c>
@@ -15010,8 +14885,17 @@
       <c r="G4" s="8">
         <v>6.4429156459154902</v>
       </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>280</v>
       </c>
@@ -15033,8 +14917,17 @@
       <c r="G5" s="8">
         <v>3.4009593119310302</v>
       </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>320</v>
       </c>
@@ -15056,8 +14949,17 @@
       <c r="G6" s="8">
         <v>2.4363095817896099</v>
       </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>360</v>
       </c>
@@ -15079,8 +14981,17 @@
       <c r="G7" s="8">
         <v>2.1643141369056398</v>
       </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>400</v>
       </c>
@@ -15102,8 +15013,17 @@
       <c r="G8" s="8">
         <v>2.1967323589023602</v>
       </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>440</v>
       </c>
@@ -15125,8 +15045,17 @@
       <c r="G9" s="8">
         <v>2.15821763569675</v>
       </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>480</v>
       </c>
@@ -15148,8 +15077,17 @@
       <c r="G10" s="8">
         <v>2.19944143780836</v>
       </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>520</v>
       </c>
@@ -15171,8 +15109,17 @@
       <c r="G11" s="8">
         <v>2.18471846914899</v>
       </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>560</v>
       </c>
@@ -15194,8 +15141,17 @@
       <c r="G12" s="8">
         <v>2.1986445153728802</v>
       </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>600</v>
       </c>
@@ -15217,8 +15173,17 @@
       <c r="G13" s="8">
         <v>2.20296187623845</v>
       </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>640</v>
       </c>
@@ -15240,8 +15205,17 @@
       <c r="G14" s="8">
         <v>2.1994092317612699</v>
       </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>680</v>
       </c>
@@ -15263,8 +15237,17 @@
       <c r="G15" s="8">
         <v>2.20021136956119</v>
       </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>720</v>
       </c>
@@ -15286,8 +15269,17 @@
       <c r="G16" s="8">
         <v>2.2008451582039701</v>
       </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>760</v>
       </c>
@@ -15309,8 +15301,17 @@
       <c r="G17" s="8">
         <v>2.2006481796600599</v>
       </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>800</v>
       </c>
@@ -15326,8 +15327,17 @@
       <c r="E18" s="6">
         <v>180</v>
       </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>840</v>
       </c>
@@ -15343,8 +15353,17 @@
       <c r="E19" s="6">
         <v>174</v>
       </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>880</v>
       </c>
@@ -15360,8 +15379,17 @@
       <c r="E20" s="6">
         <v>162</v>
       </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>920</v>
       </c>
@@ -15377,8 +15405,17 @@
       <c r="E21" s="6">
         <v>156</v>
       </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>960</v>
       </c>
@@ -15394,8 +15431,17 @@
       <c r="E22" s="6">
         <v>150</v>
       </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1000</v>
       </c>
@@ -15414,7 +15460,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -15439,7 +15485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E62CD7-0F75-45A2-BA1A-AFAB0AA7A42B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>

</xml_diff>